<commit_message>
more wrangling inorganic n extraction data
</commit_message>
<xml_diff>
--- a/Soil-Data-Raw-R/Soil-Data-RawFolders/Soil N Extractions/Extraction calcs practice/prac2.xlsx
+++ b/Soil-Data-Raw-R/Soil-Data-RawFolders/Soil N Extractions/Extraction calcs practice/prac2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="70">
   <si>
     <t>Site</t>
   </si>
@@ -290,7 +290,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="121">
+  <cellStyleXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -412,8 +412,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -427,8 +429,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="121">
+  <cellStyles count="123">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -489,6 +492,7 @@
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -549,6 +553,7 @@
     <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -878,13 +883,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF42"/>
+  <dimension ref="A1:AG42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB26" sqref="AB26"/>
+      <selection pane="bottomRight" activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -903,22 +908,22 @@
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.1640625" customWidth="1"/>
-    <col min="18" max="19" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="33.83203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="11.1640625" customWidth="1"/>
+    <col min="19" max="20" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -967,32 +972,35 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:25">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -1044,36 +1052,38 @@
       <c r="P2">
         <v>2.6859999999999999</v>
       </c>
-      <c r="R2">
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2">
         <f>O2*$N2</f>
         <v>5.4771072342426327E-2</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <f>P2*$N2</f>
         <v>0.14021645092618865</v>
       </c>
-      <c r="T2" s="5">
-        <f>SUM(R2:S2)</f>
+      <c r="U2" s="5">
+        <f>SUM(S2:T2)</f>
         <v>0.19498752326861496</v>
       </c>
-      <c r="U2">
-        <f>(K2/J2)*H2</f>
+      <c r="V2">
+        <f t="shared" ref="V2:V21" si="0">(K2/J2)*H2</f>
         <v>8.0973004742410133</v>
       </c>
-      <c r="V2">
-        <f>R2/$U2</f>
+      <c r="W2">
+        <f>S2/$V2</f>
         <v>6.7641150920190107E-3</v>
       </c>
-      <c r="W2">
-        <f>S2/$U2</f>
+      <c r="X2">
+        <f>T2/$V2</f>
         <v>1.7316444088031895E-2</v>
       </c>
-      <c r="X2" s="5">
-        <f>T2/$U2</f>
+      <c r="Y2" s="5">
+        <f>U2/$V2</f>
         <v>2.4080559180050903E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:25">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -1112,11 +1122,11 @@
         <v>2.0762478021772468</v>
       </c>
       <c r="M3" s="2">
-        <f t="shared" ref="M3:M27" si="0">L3*0.001</f>
+        <f t="shared" ref="M3:M21" si="1">L3*0.001</f>
         <v>2.0762478021772468E-3</v>
       </c>
       <c r="N3" s="2">
-        <f t="shared" ref="N3:N11" si="1">M3+(I3*0.001)</f>
+        <f t="shared" ref="N3:N11" si="2">M3+(I3*0.001)</f>
         <v>5.2076247802177247E-2</v>
       </c>
       <c r="O3">
@@ -1125,36 +1135,38 @@
       <c r="P3">
         <v>0.66600000000000004</v>
       </c>
-      <c r="R3">
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3">
         <f>O3*$N3</f>
         <v>4.8698738598471437E-2</v>
       </c>
-      <c r="S3">
-        <f t="shared" ref="S3:S24" si="2">P3*$N3</f>
+      <c r="T3">
+        <f t="shared" ref="T3:T24" si="3">P3*$N3</f>
         <v>3.4682781036250047E-2</v>
       </c>
-      <c r="T3" s="5">
-        <f>SUM(R3:S3)</f>
+      <c r="U3" s="5">
+        <f>SUM(S3:T3)</f>
         <v>8.3381519634721485E-2</v>
       </c>
-      <c r="U3">
-        <f>(K3/J3)*H3</f>
+      <c r="V3">
+        <f t="shared" si="0"/>
         <v>7.7537521978227533</v>
       </c>
-      <c r="V3">
-        <f>R3/$U3</f>
+      <c r="W3">
+        <f>S3/$V3</f>
         <v>6.2806673925104289E-3</v>
       </c>
-      <c r="W3">
-        <f t="shared" ref="W3:W21" si="3">S3/$U3</f>
+      <c r="X3">
+        <f t="shared" ref="X3:X21" si="4">T3/$V3</f>
         <v>4.4730319142761545E-3</v>
       </c>
-      <c r="X3" s="5">
-        <f t="shared" ref="X3:X21" si="4">T3/$U3</f>
+      <c r="Y3" s="5">
+        <f t="shared" ref="Y3:Y21" si="5">U3/$V3</f>
         <v>1.0753699306786582E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:25">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -1189,15 +1201,15 @@
         <v>277.45</v>
       </c>
       <c r="L4" s="2">
-        <f t="shared" ref="L4:L11" si="5">H4-((1-((J4-K4)/J4))*H4)</f>
+        <f t="shared" ref="L4:L11" si="6">H4-((1-((J4-K4)/J4))*H4)</f>
         <v>2.165478448155298</v>
       </c>
       <c r="M4" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.1654784481552982E-3</v>
       </c>
       <c r="N4" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.2165478448155299E-2</v>
       </c>
       <c r="O4">
@@ -1206,36 +1218,38 @@
       <c r="P4">
         <v>2.4710000000000001</v>
       </c>
-      <c r="R4">
-        <f t="shared" ref="R3:R24" si="6">O4*$N4</f>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4">
+        <f t="shared" ref="S4:S24" si="7">O4*$N4</f>
         <v>4.224360444731616E-2</v>
       </c>
-      <c r="S4">
-        <f t="shared" si="2"/>
+      <c r="T4">
+        <f t="shared" si="3"/>
         <v>0.12890089724539175</v>
       </c>
-      <c r="T4" s="5">
-        <f t="shared" ref="T3:T24" si="7">SUM(R4:S4)</f>
+      <c r="U4" s="5">
+        <f t="shared" ref="U4:U24" si="8">SUM(S4:T4)</f>
         <v>0.1711445016927079</v>
       </c>
-      <c r="U4">
-        <f>(K4/J4)*H4</f>
+      <c r="V4">
+        <f t="shared" si="0"/>
         <v>7.5045215518447028</v>
       </c>
-      <c r="V4">
-        <f t="shared" ref="V3:V21" si="8">R4/$U4</f>
+      <c r="W4">
+        <f t="shared" ref="W4:W21" si="9">S4/$V4</f>
         <v>5.6290869651686413E-3</v>
       </c>
-      <c r="W4">
-        <f t="shared" si="3"/>
+      <c r="X4">
+        <f t="shared" si="4"/>
         <v>1.7176431082899127E-2</v>
       </c>
-      <c r="X4" s="5">
-        <f t="shared" si="4"/>
+      <c r="Y4" s="5">
+        <f t="shared" si="5"/>
         <v>2.2805518048067765E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:25">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -1270,15 +1284,15 @@
         <v>290.15000000000003</v>
       </c>
       <c r="L5" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.187843657895435</v>
       </c>
       <c r="M5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.1878436578954353E-3</v>
       </c>
       <c r="N5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.2187843657895437E-2</v>
       </c>
       <c r="O5">
@@ -1287,36 +1301,38 @@
       <c r="P5">
         <v>4.0129999999999999</v>
       </c>
-      <c r="R5">
-        <f t="shared" si="6"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5">
+        <f t="shared" si="7"/>
         <v>0.12391742537348982</v>
       </c>
-      <c r="S5">
-        <f t="shared" si="2"/>
+      <c r="T5">
+        <f t="shared" si="3"/>
         <v>0.20942981659913437</v>
       </c>
-      <c r="T5" s="5">
-        <f t="shared" si="7"/>
+      <c r="U5" s="5">
+        <f t="shared" si="8"/>
         <v>0.33334724197262422</v>
       </c>
-      <c r="U5">
-        <f>(K5/J5)*H5</f>
+      <c r="V5">
+        <f t="shared" si="0"/>
         <v>7.3421563421045644</v>
       </c>
-      <c r="V5">
-        <f t="shared" si="8"/>
+      <c r="W5">
+        <f t="shared" si="9"/>
         <v>1.6877524748808329E-2</v>
       </c>
-      <c r="W5">
-        <f t="shared" si="3"/>
+      <c r="X5">
+        <f t="shared" si="4"/>
         <v>2.8524292706507959E-2</v>
       </c>
-      <c r="X5" s="5">
-        <f t="shared" si="4"/>
+      <c r="Y5" s="5">
+        <f t="shared" si="5"/>
         <v>4.5401817455316289E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:25">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -1351,15 +1367,15 @@
         <v>372.65000000000003</v>
       </c>
       <c r="L6" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.1728513114651156</v>
       </c>
       <c r="M6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.1728513114651158E-3</v>
       </c>
       <c r="N6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.2172851311465117E-2</v>
       </c>
       <c r="O6">
@@ -1368,36 +1384,38 @@
       <c r="P6">
         <v>1.1759999999999999</v>
       </c>
-      <c r="R6">
-        <f t="shared" si="6"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6">
+        <f t="shared" si="7"/>
         <v>6.0984845897971575E-2</v>
       </c>
-      <c r="S6">
-        <f t="shared" si="2"/>
+      <c r="T6">
+        <f t="shared" si="3"/>
         <v>6.1355273142282972E-2</v>
       </c>
-      <c r="T6" s="5">
-        <f t="shared" si="7"/>
+      <c r="U6" s="5">
+        <f t="shared" si="8"/>
         <v>0.12234011904025455</v>
       </c>
-      <c r="U6">
-        <f>(K6/J6)*H6</f>
+      <c r="V6">
+        <f t="shared" si="0"/>
         <v>7.7071486885348852</v>
       </c>
-      <c r="V6">
-        <f t="shared" si="8"/>
+      <c r="W6">
+        <f t="shared" si="9"/>
         <v>7.9127636383468664E-3</v>
       </c>
-      <c r="W6">
-        <f t="shared" si="3"/>
+      <c r="X6">
+        <f t="shared" si="4"/>
         <v>7.9608264511043837E-3</v>
       </c>
-      <c r="X6" s="5">
-        <f t="shared" si="4"/>
+      <c r="Y6" s="5">
+        <f t="shared" si="5"/>
         <v>1.5873590089451248E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:25">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -1432,15 +1450,15 @@
         <v>441.95</v>
       </c>
       <c r="L7" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.6750423896829734</v>
       </c>
       <c r="M7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.6750423896829735E-3</v>
       </c>
       <c r="N7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.1675042389682978E-2</v>
       </c>
       <c r="O7">
@@ -1449,36 +1467,38 @@
       <c r="P7">
         <v>0.36899999999999999</v>
       </c>
-      <c r="R7">
-        <f t="shared" si="6"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7">
+        <f t="shared" si="7"/>
         <v>6.6588459623345489E-2</v>
       </c>
-      <c r="S7">
-        <f t="shared" si="2"/>
+      <c r="T7">
+        <f t="shared" si="3"/>
         <v>1.9068090641793017E-2</v>
       </c>
-      <c r="T7" s="5">
-        <f t="shared" si="7"/>
+      <c r="U7" s="5">
+        <f t="shared" si="8"/>
         <v>8.5656550265138506E-2</v>
       </c>
-      <c r="U7">
-        <f>(K7/J7)*H7</f>
+      <c r="V7">
+        <f t="shared" si="0"/>
         <v>8.4449576103170259</v>
       </c>
-      <c r="V7">
-        <f t="shared" si="8"/>
+      <c r="W7">
+        <f t="shared" si="9"/>
         <v>7.8849963133024829E-3</v>
       </c>
-      <c r="W7">
-        <f t="shared" si="3"/>
+      <c r="X7">
+        <f t="shared" si="4"/>
         <v>2.2579261521097436E-3</v>
       </c>
-      <c r="X7" s="5">
-        <f t="shared" si="4"/>
+      <c r="Y7" s="5">
+        <f t="shared" si="5"/>
         <v>1.0142922465412227E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:25">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -1513,15 +1533,15 @@
         <v>439.95</v>
       </c>
       <c r="L8" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.6932847548562631</v>
       </c>
       <c r="M8" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.6932847548562632E-3</v>
       </c>
       <c r="N8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.1693284754856267E-2</v>
       </c>
       <c r="O8">
@@ -1530,36 +1550,38 @@
       <c r="P8">
         <v>0.39900000000000002</v>
       </c>
-      <c r="R8">
-        <f t="shared" si="6"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8">
+        <f t="shared" si="7"/>
         <v>0.12495300790943856</v>
       </c>
-      <c r="S8">
-        <f t="shared" si="2"/>
+      <c r="T8">
+        <f t="shared" si="3"/>
         <v>2.0625620617187652E-2</v>
       </c>
-      <c r="T8" s="5">
-        <f t="shared" si="7"/>
+      <c r="U8" s="5">
+        <f t="shared" si="8"/>
         <v>0.1455786285266262</v>
       </c>
-      <c r="U8">
-        <f>(K8/J8)*H8</f>
+      <c r="V8">
+        <f t="shared" si="0"/>
         <v>8.6967152451437375</v>
       </c>
-      <c r="V8">
-        <f t="shared" si="8"/>
+      <c r="W8">
+        <f t="shared" si="9"/>
         <v>1.4367839395363962E-2</v>
       </c>
-      <c r="W8">
-        <f t="shared" si="3"/>
+      <c r="X8">
+        <f t="shared" si="4"/>
         <v>2.3716564284089947E-3</v>
       </c>
-      <c r="X8" s="5">
-        <f t="shared" si="4"/>
+      <c r="Y8" s="5">
+        <f t="shared" si="5"/>
         <v>1.6739495823772956E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:25">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -1594,15 +1616,15 @@
         <v>224.15</v>
       </c>
       <c r="L9" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.5506585484292712</v>
       </c>
       <c r="M9" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5506585484292713E-3</v>
       </c>
       <c r="N9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.1550658548429273E-2</v>
       </c>
       <c r="O9">
@@ -1611,36 +1633,38 @@
       <c r="P9">
         <v>0.36499999999999999</v>
       </c>
-      <c r="R9">
-        <f t="shared" si="6"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9">
+        <f t="shared" si="7"/>
         <v>0.11270778231735834</v>
       </c>
-      <c r="S9">
-        <f t="shared" si="2"/>
+      <c r="T9">
+        <f t="shared" si="3"/>
         <v>1.8815990370176686E-2</v>
       </c>
-      <c r="T9" s="5">
-        <f t="shared" si="7"/>
+      <c r="U9" s="5">
+        <f t="shared" si="8"/>
         <v>0.13152377268753501</v>
       </c>
-      <c r="U9">
-        <f>(K9/J9)*H9</f>
+      <c r="V9">
+        <f t="shared" si="0"/>
         <v>7.9793414515707282</v>
       </c>
-      <c r="V9">
-        <f t="shared" si="8"/>
+      <c r="W9">
+        <f t="shared" si="9"/>
         <v>1.4124947904713601E-2</v>
       </c>
-      <c r="W9">
-        <f t="shared" si="3"/>
+      <c r="X9">
+        <f t="shared" si="4"/>
         <v>2.3580881310039403E-3</v>
       </c>
-      <c r="X9" s="5">
-        <f t="shared" si="4"/>
+      <c r="Y9" s="5">
+        <f t="shared" si="5"/>
         <v>1.648303603571754E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:25">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -1675,15 +1699,15 @@
         <v>462.65000000000003</v>
       </c>
       <c r="L10" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.6382048646796843</v>
       </c>
       <c r="M10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.6382048646796843E-3</v>
       </c>
       <c r="N10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.1638204864679689E-2</v>
       </c>
       <c r="O10">
@@ -1692,36 +1716,38 @@
       <c r="P10">
         <v>0.33100000000000002</v>
       </c>
-      <c r="R10">
-        <f t="shared" si="6"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10">
+        <f t="shared" si="7"/>
         <v>0.10936713599314835</v>
       </c>
-      <c r="S10">
-        <f t="shared" si="2"/>
+      <c r="T10">
+        <f t="shared" si="3"/>
         <v>1.7092245810208979E-2</v>
       </c>
-      <c r="T10" s="5">
-        <f t="shared" si="7"/>
+      <c r="U10" s="5">
+        <f t="shared" si="8"/>
         <v>0.12645938180335733</v>
       </c>
-      <c r="U10">
-        <f>(K10/J10)*H10</f>
+      <c r="V10">
+        <f t="shared" si="0"/>
         <v>8.2417951353203165</v>
       </c>
-      <c r="V10">
-        <f t="shared" si="8"/>
+      <c r="W10">
+        <f t="shared" si="9"/>
         <v>1.3269819765897129E-2</v>
       </c>
-      <c r="W10">
-        <f t="shared" si="3"/>
+      <c r="X10">
+        <f t="shared" si="4"/>
         <v>2.073849874884653E-3</v>
       </c>
-      <c r="X10" s="5">
-        <f t="shared" si="4"/>
+      <c r="Y10" s="5">
+        <f t="shared" si="5"/>
         <v>1.5343669640781784E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:25">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -1756,15 +1782,15 @@
         <v>484.75</v>
       </c>
       <c r="L11" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.7364177221663457</v>
       </c>
       <c r="M11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.7364177221663457E-3</v>
       </c>
       <c r="N11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.1736417722166347E-2</v>
       </c>
       <c r="O11">
@@ -1773,36 +1799,38 @@
       <c r="P11">
         <v>0.29599999999999999</v>
       </c>
-      <c r="R11">
-        <f t="shared" si="6"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11">
+        <f t="shared" si="7"/>
         <v>0.13099660967252519</v>
       </c>
-      <c r="S11">
-        <f t="shared" si="2"/>
+      <c r="T11">
+        <f t="shared" si="3"/>
         <v>1.5313979645761238E-2</v>
       </c>
-      <c r="T11" s="5">
-        <f t="shared" si="7"/>
+      <c r="U11" s="5">
+        <f t="shared" si="8"/>
         <v>0.14631058931828642</v>
       </c>
-      <c r="U11">
-        <f>(K11/J11)*H11</f>
+      <c r="V11">
+        <f t="shared" si="0"/>
         <v>8.2635822778336543</v>
       </c>
-      <c r="V11">
-        <f t="shared" si="8"/>
+      <c r="W11">
+        <f t="shared" si="9"/>
         <v>1.5852278741619392E-2</v>
       </c>
-      <c r="W11">
-        <f t="shared" si="3"/>
+      <c r="X11">
+        <f t="shared" si="4"/>
         <v>1.8531889840123774E-3</v>
       </c>
-      <c r="X11" s="5">
-        <f t="shared" si="4"/>
+      <c r="Y11" s="5">
+        <f t="shared" si="5"/>
         <v>1.7705467725631769E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -1854,36 +1882,38 @@
       <c r="P12">
         <v>0.38275120000000001</v>
       </c>
-      <c r="R12">
-        <f t="shared" si="6"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12">
+        <f t="shared" si="7"/>
         <v>0.18008182613294962</v>
       </c>
-      <c r="S12">
-        <f t="shared" si="2"/>
+      <c r="T12">
+        <f t="shared" si="3"/>
         <v>1.9914344957767744E-2</v>
       </c>
-      <c r="T12" s="5">
-        <f t="shared" si="7"/>
+      <c r="U12" s="5">
+        <f t="shared" si="8"/>
         <v>0.19999617109071738</v>
       </c>
-      <c r="U12">
-        <f>(K12/J12)*H12</f>
+      <c r="V12">
+        <f t="shared" si="0"/>
         <v>7.460522475781282</v>
       </c>
-      <c r="V12">
-        <f t="shared" si="8"/>
+      <c r="W12">
+        <f t="shared" si="9"/>
         <v>2.4137964427764971E-2</v>
       </c>
-      <c r="W12">
-        <f t="shared" si="3"/>
+      <c r="X12">
+        <f t="shared" si="4"/>
         <v>2.6692962888879E-3</v>
       </c>
-      <c r="X12" s="5">
-        <f t="shared" si="4"/>
+      <c r="Y12" s="5">
+        <f t="shared" si="5"/>
         <v>2.6807260716652872E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:25">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
@@ -1922,11 +1952,11 @@
         <v>2.1522853615652231</v>
       </c>
       <c r="M13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.1522853615652229E-3</v>
       </c>
       <c r="N13" s="2">
-        <f t="shared" ref="N13:N21" si="9">M13+(I13*0.001)</f>
+        <f t="shared" ref="N13:N21" si="10">M13+(I13*0.001)</f>
         <v>5.2152285361565229E-2</v>
       </c>
       <c r="O13">
@@ -1935,36 +1965,38 @@
       <c r="P13">
         <v>0.49849759999999999</v>
       </c>
-      <c r="R13">
-        <f t="shared" si="6"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13">
+        <f t="shared" si="7"/>
         <v>0.14277731163435711</v>
       </c>
-      <c r="S13">
-        <f t="shared" si="2"/>
+      <c r="T13">
+        <f t="shared" si="3"/>
         <v>2.5997789087255398E-2</v>
       </c>
-      <c r="T13" s="5">
-        <f t="shared" si="7"/>
+      <c r="U13" s="5">
+        <f t="shared" si="8"/>
         <v>0.1687751007216125</v>
       </c>
-      <c r="U13">
-        <f>(K13/J13)*H13</f>
+      <c r="V13">
+        <f t="shared" si="0"/>
         <v>8.0377146384347764</v>
       </c>
-      <c r="V13">
-        <f t="shared" si="8"/>
+      <c r="W13">
+        <f t="shared" si="9"/>
         <v>1.7763421327702276E-2</v>
       </c>
-      <c r="W13">
-        <f t="shared" si="3"/>
+      <c r="X13">
+        <f t="shared" si="4"/>
         <v>3.234475252821127E-3</v>
       </c>
-      <c r="X13" s="5">
-        <f t="shared" si="4"/>
+      <c r="Y13" s="5">
+        <f t="shared" si="5"/>
         <v>2.0997896580523406E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:25">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
@@ -1999,15 +2031,15 @@
         <v>277.45</v>
       </c>
       <c r="L14" s="2">
-        <f t="shared" ref="L14:L22" si="10">H14-((1-((J14-K14)/J14))*H14)</f>
+        <f t="shared" ref="L14:L21" si="11">H14-((1-((J14-K14)/J14))*H14)</f>
         <v>2.2348991636597599</v>
       </c>
       <c r="M14" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.23489916365976E-3</v>
       </c>
       <c r="N14" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.2234899163659761E-2</v>
       </c>
       <c r="O14">
@@ -2016,36 +2048,38 @@
       <c r="P14">
         <v>0.55169800000000002</v>
       </c>
-      <c r="R14">
-        <f t="shared" si="6"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14">
+        <f t="shared" si="7"/>
         <v>0.22730277545562361</v>
       </c>
-      <c r="S14">
-        <f t="shared" si="2"/>
+      <c r="T14">
+        <f t="shared" si="3"/>
         <v>2.8817889398792765E-2</v>
       </c>
-      <c r="T14" s="5">
-        <f t="shared" si="7"/>
+      <c r="U14" s="5">
+        <f t="shared" si="8"/>
         <v>0.25612066485441637</v>
       </c>
-      <c r="U14">
-        <f>(K14/J14)*H14</f>
+      <c r="V14">
+        <f t="shared" si="0"/>
         <v>7.7451008363402414</v>
       </c>
-      <c r="V14">
-        <f t="shared" si="8"/>
+      <c r="W14">
+        <f t="shared" si="9"/>
         <v>2.9347942687732647E-2</v>
       </c>
-      <c r="W14">
-        <f t="shared" si="3"/>
+      <c r="X14">
+        <f t="shared" si="4"/>
         <v>3.7207894393806182E-3</v>
       </c>
-      <c r="X14" s="5">
-        <f t="shared" si="4"/>
+      <c r="Y14" s="5">
+        <f t="shared" si="5"/>
         <v>3.3068732127113268E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:25">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
@@ -2080,15 +2114,15 @@
         <v>290.15000000000003</v>
       </c>
       <c r="L15" s="2">
+        <f t="shared" si="11"/>
+        <v>2.1993223759326623</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="1"/>
+        <v>2.1993223759326623E-3</v>
+      </c>
+      <c r="N15" s="2">
         <f t="shared" si="10"/>
-        <v>2.1993223759326623</v>
-      </c>
-      <c r="M15" s="2">
-        <f t="shared" si="0"/>
-        <v>2.1993223759326623E-3</v>
-      </c>
-      <c r="N15" s="2">
-        <f t="shared" si="9"/>
         <v>5.2199322375932666E-2</v>
       </c>
       <c r="O15">
@@ -2097,36 +2131,38 @@
       <c r="P15">
         <v>0.569716</v>
       </c>
-      <c r="R15">
-        <f t="shared" si="6"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15">
+        <f t="shared" si="7"/>
         <v>0.29299218652999126</v>
       </c>
-      <c r="S15">
-        <f t="shared" si="2"/>
+      <c r="T15">
+        <f t="shared" si="3"/>
         <v>2.9738789146726854E-2</v>
       </c>
-      <c r="T15" s="5">
-        <f t="shared" si="7"/>
+      <c r="U15" s="5">
+        <f t="shared" si="8"/>
         <v>0.3227309756767181</v>
       </c>
-      <c r="U15">
-        <f>(K15/J15)*H15</f>
+      <c r="V15">
+        <f t="shared" si="0"/>
         <v>7.3806776240673377</v>
       </c>
-      <c r="V15">
-        <f t="shared" si="8"/>
+      <c r="W15">
+        <f t="shared" si="9"/>
         <v>3.9697193327423691E-2</v>
       </c>
-      <c r="W15">
-        <f t="shared" si="3"/>
+      <c r="X15">
+        <f t="shared" si="4"/>
         <v>4.0292762618100138E-3</v>
       </c>
-      <c r="X15" s="5">
-        <f t="shared" si="4"/>
+      <c r="Y15" s="5">
+        <f t="shared" si="5"/>
         <v>4.37264695892337E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:25">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -2161,15 +2197,15 @@
         <v>372.65000000000003</v>
       </c>
       <c r="L16" s="2">
+        <f t="shared" si="11"/>
+        <v>2.293809633459631</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" si="1"/>
+        <v>2.2938096334596311E-3</v>
+      </c>
+      <c r="N16" s="2">
         <f t="shared" si="10"/>
-        <v>2.293809633459631</v>
-      </c>
-      <c r="M16" s="2">
-        <f t="shared" si="0"/>
-        <v>2.2938096334596311E-3</v>
-      </c>
-      <c r="N16" s="2">
-        <f t="shared" si="9"/>
         <v>5.2293809633459636E-2</v>
       </c>
       <c r="O16">
@@ -2178,36 +2214,38 @@
       <c r="P16">
         <v>0.6237568</v>
       </c>
-      <c r="R16">
-        <f t="shared" si="6"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16">
+        <f t="shared" si="7"/>
         <v>0.18196676938154949</v>
       </c>
-      <c r="S16">
-        <f t="shared" si="2"/>
+      <c r="T16">
+        <f t="shared" si="3"/>
         <v>3.2618619356775957E-2</v>
       </c>
-      <c r="T16" s="5">
-        <f t="shared" si="7"/>
+      <c r="U16" s="5">
+        <f t="shared" si="8"/>
         <v>0.21458538873832544</v>
       </c>
-      <c r="U16">
-        <f>(K16/J16)*H16</f>
+      <c r="V16">
+        <f t="shared" si="0"/>
         <v>8.1361903665403688</v>
       </c>
-      <c r="V16">
-        <f t="shared" si="8"/>
+      <c r="W16">
+        <f t="shared" si="9"/>
         <v>2.2365107155048598E-2</v>
       </c>
-      <c r="W16">
-        <f t="shared" si="3"/>
+      <c r="X16">
+        <f t="shared" si="4"/>
         <v>4.0090776994253013E-3</v>
       </c>
-      <c r="X16" s="5">
-        <f t="shared" si="4"/>
+      <c r="Y16" s="5">
+        <f t="shared" si="5"/>
         <v>2.63741848544739E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:32">
+    <row r="17" spans="1:33">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -2242,15 +2280,15 @@
         <v>441.95</v>
       </c>
       <c r="L17" s="2">
+        <f t="shared" si="11"/>
+        <v>1.699870093087366</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" si="1"/>
+        <v>1.699870093087366E-3</v>
+      </c>
+      <c r="N17" s="2">
         <f t="shared" si="10"/>
-        <v>1.699870093087366</v>
-      </c>
-      <c r="M17" s="2">
-        <f t="shared" si="0"/>
-        <v>1.699870093087366E-3</v>
-      </c>
-      <c r="N17" s="2">
-        <f t="shared" si="9"/>
         <v>5.1699870093087366E-2</v>
       </c>
       <c r="O17">
@@ -2259,36 +2297,38 @@
       <c r="P17">
         <v>0.32879839999999999</v>
       </c>
-      <c r="R17">
-        <f t="shared" si="6"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17">
+        <f t="shared" si="7"/>
         <v>0.12427614772976341</v>
       </c>
-      <c r="S17">
-        <f t="shared" si="2"/>
+      <c r="T17">
+        <f t="shared" si="3"/>
         <v>1.6998834566814978E-2</v>
       </c>
-      <c r="T17" s="5">
-        <f t="shared" si="7"/>
+      <c r="U17" s="5">
+        <f t="shared" si="8"/>
         <v>0.14127498229657839</v>
       </c>
-      <c r="U17">
-        <f>(K17/J17)*H17</f>
+      <c r="V17">
+        <f t="shared" si="0"/>
         <v>8.5701299069126335</v>
       </c>
-      <c r="V17">
-        <f t="shared" si="8"/>
+      <c r="W17">
+        <f t="shared" si="9"/>
         <v>1.4501080973057683E-2</v>
       </c>
-      <c r="W17">
-        <f t="shared" si="3"/>
+      <c r="X17">
+        <f t="shared" si="4"/>
         <v>1.9834978875995549E-3</v>
       </c>
-      <c r="X17" s="5">
-        <f t="shared" si="4"/>
+      <c r="Y17" s="5">
+        <f t="shared" si="5"/>
         <v>1.648457886065724E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:32">
+    <row r="18" spans="1:33">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -2323,15 +2363,15 @@
         <v>439.95</v>
       </c>
       <c r="L18" s="2">
+        <f t="shared" si="11"/>
+        <v>1.6916550293944184</v>
+      </c>
+      <c r="M18" s="2">
+        <f t="shared" si="1"/>
+        <v>1.6916550293944183E-3</v>
+      </c>
+      <c r="N18" s="2">
         <f t="shared" si="10"/>
-        <v>1.6916550293944184</v>
-      </c>
-      <c r="M18" s="2">
-        <f t="shared" si="0"/>
-        <v>1.6916550293944183E-3</v>
-      </c>
-      <c r="N18" s="2">
-        <f t="shared" si="9"/>
         <v>5.169165502939442E-2</v>
       </c>
       <c r="O18">
@@ -2340,36 +2380,38 @@
       <c r="P18">
         <v>0.41092879999999998</v>
       </c>
-      <c r="R18">
-        <f t="shared" si="6"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18">
+        <f t="shared" si="7"/>
         <v>0.15494056678510681</v>
       </c>
-      <c r="S18">
-        <f t="shared" si="2"/>
+      <c r="T18">
+        <f t="shared" si="3"/>
         <v>2.1241589771243012E-2</v>
       </c>
-      <c r="T18" s="5">
-        <f t="shared" si="7"/>
+      <c r="U18" s="5">
+        <f t="shared" si="8"/>
         <v>0.17618215655634983</v>
       </c>
-      <c r="U18">
-        <f>(K18/J18)*H18</f>
+      <c r="V18">
+        <f t="shared" si="0"/>
         <v>8.6883449706055824</v>
       </c>
-      <c r="V18">
-        <f t="shared" si="8"/>
+      <c r="W18">
+        <f t="shared" si="9"/>
         <v>1.7833150883085548E-2</v>
       </c>
-      <c r="W18">
-        <f t="shared" si="3"/>
+      <c r="X18">
+        <f t="shared" si="4"/>
         <v>2.4448372898529676E-3</v>
       </c>
-      <c r="X18" s="5">
-        <f t="shared" si="4"/>
+      <c r="Y18" s="5">
+        <f t="shared" si="5"/>
         <v>2.0277988172938514E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:32">
+    <row r="19" spans="1:33">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -2404,15 +2446,15 @@
         <v>224.15</v>
       </c>
       <c r="L19" s="2">
+        <f t="shared" si="11"/>
+        <v>1.5587942176235483</v>
+      </c>
+      <c r="M19" s="2">
+        <f t="shared" si="1"/>
+        <v>1.5587942176235484E-3</v>
+      </c>
+      <c r="N19" s="2">
         <f t="shared" si="10"/>
-        <v>1.5587942176235483</v>
-      </c>
-      <c r="M19" s="2">
-        <f t="shared" si="0"/>
-        <v>1.5587942176235484E-3</v>
-      </c>
-      <c r="N19" s="2">
-        <f t="shared" si="9"/>
         <v>5.1558794217623549E-2</v>
       </c>
       <c r="O19">
@@ -2421,40 +2463,42 @@
       <c r="P19">
         <v>0.29482160000000002</v>
       </c>
-      <c r="R19">
-        <f t="shared" si="6"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19">
+        <f t="shared" si="7"/>
         <v>0.15836799231885251</v>
       </c>
-      <c r="S19">
-        <f t="shared" si="2"/>
+      <c r="T19">
+        <f t="shared" si="3"/>
         <v>1.5200646205310524E-2</v>
       </c>
-      <c r="T19" s="5">
-        <f t="shared" si="7"/>
+      <c r="U19" s="5">
+        <f t="shared" si="8"/>
         <v>0.17356863852416304</v>
       </c>
-      <c r="U19">
-        <f>(K19/J19)*H19</f>
+      <c r="V19">
+        <f t="shared" si="0"/>
         <v>8.0212057823764518</v>
       </c>
-      <c r="V19">
-        <f t="shared" si="8"/>
+      <c r="W19">
+        <f t="shared" si="9"/>
         <v>1.974366405943679E-2</v>
       </c>
-      <c r="W19">
-        <f t="shared" si="3"/>
+      <c r="X19">
+        <f t="shared" si="4"/>
         <v>1.8950575035374558E-3</v>
       </c>
-      <c r="X19" s="5">
-        <f t="shared" si="4"/>
+      <c r="Y19" s="5">
+        <f t="shared" si="5"/>
         <v>2.1638721562974247E-2</v>
       </c>
-      <c r="AC19">
-        <f>SUM(AA33:AB33)</f>
+      <c r="AD19">
+        <f>SUM(AB33:AC33)</f>
         <v>3.895287909431379E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:32">
+    <row r="20" spans="1:33">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -2489,15 +2533,15 @@
         <v>462.65000000000003</v>
       </c>
       <c r="L20" s="2">
+        <f t="shared" si="11"/>
+        <v>1.5917780061664946</v>
+      </c>
+      <c r="M20" s="2">
+        <f t="shared" si="1"/>
+        <v>1.5917780061664947E-3</v>
+      </c>
+      <c r="N20" s="2">
         <f t="shared" si="10"/>
-        <v>1.5917780061664946</v>
-      </c>
-      <c r="M20" s="2">
-        <f t="shared" si="0"/>
-        <v>1.5917780061664947E-3</v>
-      </c>
-      <c r="N20" s="2">
-        <f t="shared" si="9"/>
         <v>5.1591778006166496E-2</v>
       </c>
       <c r="O20">
@@ -2506,36 +2550,38 @@
       <c r="P20">
         <v>0.36457919999999999</v>
       </c>
-      <c r="R20">
-        <f t="shared" si="6"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20">
+        <f t="shared" si="7"/>
         <v>0.20536365194244605</v>
       </c>
-      <c r="S20">
-        <f t="shared" si="2"/>
+      <c r="T20">
+        <f t="shared" si="3"/>
         <v>1.8809289152065777E-2</v>
       </c>
-      <c r="T20" s="5">
-        <f t="shared" si="7"/>
+      <c r="U20" s="5">
+        <f t="shared" si="8"/>
         <v>0.22417294109451183</v>
       </c>
-      <c r="U20">
-        <f>(K20/J20)*H20</f>
+      <c r="V20">
+        <f t="shared" si="0"/>
         <v>8.0082219938335051</v>
       </c>
-      <c r="V20">
-        <f t="shared" si="8"/>
+      <c r="W20">
+        <f t="shared" si="9"/>
         <v>2.5644100787987678E-2</v>
       </c>
-      <c r="W20">
-        <f t="shared" si="3"/>
+      <c r="X20">
+        <f t="shared" si="4"/>
         <v>2.348747220862423E-3</v>
       </c>
-      <c r="X20" s="5">
-        <f t="shared" si="4"/>
+      <c r="Y20" s="5">
+        <f t="shared" si="5"/>
         <v>2.7992848008850102E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:32">
+    <row r="21" spans="1:33">
       <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
@@ -2570,15 +2616,15 @@
         <v>484.75</v>
       </c>
       <c r="L21" s="2">
+        <f t="shared" si="11"/>
+        <v>1.6982165322786855</v>
+      </c>
+      <c r="M21" s="2">
+        <f t="shared" si="1"/>
+        <v>1.6982165322786855E-3</v>
+      </c>
+      <c r="N21" s="2">
         <f t="shared" si="10"/>
-        <v>1.6982165322786855</v>
-      </c>
-      <c r="M21" s="2">
-        <f t="shared" si="0"/>
-        <v>1.6982165322786855E-3</v>
-      </c>
-      <c r="N21" s="2">
-        <f t="shared" si="9"/>
         <v>5.1698216532278692E-2</v>
       </c>
       <c r="O21">
@@ -2587,36 +2633,38 @@
       <c r="P21">
         <v>0.31357879999999999</v>
       </c>
-      <c r="R21">
-        <f t="shared" si="6"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21">
+        <f t="shared" si="7"/>
         <v>0.13641313716538145</v>
       </c>
-      <c r="S21">
-        <f t="shared" si="2"/>
+      <c r="T21">
+        <f t="shared" si="3"/>
         <v>1.6211464702332114E-2</v>
       </c>
-      <c r="T21" s="5">
-        <f t="shared" si="7"/>
+      <c r="U21" s="5">
+        <f t="shared" si="8"/>
         <v>0.15262460186771357</v>
       </c>
-      <c r="U21">
-        <f>(K21/J21)*H21</f>
+      <c r="V21">
+        <f t="shared" si="0"/>
         <v>8.0817834677213138</v>
       </c>
-      <c r="V21">
-        <f t="shared" si="8"/>
+      <c r="W21">
+        <f t="shared" si="9"/>
         <v>1.6879088348532998E-2</v>
       </c>
-      <c r="W21">
-        <f t="shared" si="3"/>
+      <c r="X21">
+        <f t="shared" si="4"/>
         <v>2.0059266332834568E-3</v>
       </c>
-      <c r="X21" s="5">
-        <f t="shared" si="4"/>
+      <c r="Y21" s="5">
+        <f t="shared" si="5"/>
         <v>1.8885014981816457E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:32">
+    <row r="22" spans="1:33">
       <c r="A22" s="2" t="s">
         <v>37</v>
       </c>
@@ -2657,7 +2705,7 @@
         <v>24</v>
       </c>
       <c r="N22" s="2">
-        <f>(I22*0.001)</f>
+        <f t="shared" ref="N22:N27" si="12">(I22*0.001)</f>
         <v>0.05</v>
       </c>
       <c r="O22">
@@ -2666,21 +2714,20 @@
       <c r="P22">
         <v>0.13900000000000001</v>
       </c>
-      <c r="R22">
-        <f t="shared" si="6"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22">
+        <f t="shared" si="7"/>
         <v>3.2975000000000001E-3</v>
       </c>
-      <c r="S22">
-        <f t="shared" si="2"/>
+      <c r="T22">
+        <f t="shared" si="3"/>
         <v>6.9500000000000013E-3</v>
       </c>
-      <c r="T22" s="5">
-        <f t="shared" si="7"/>
+      <c r="U22" s="5">
+        <f t="shared" si="8"/>
         <v>1.0247500000000001E-2</v>
       </c>
-      <c r="U22" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="V22" s="4" t="s">
         <v>24</v>
       </c>
@@ -2690,8 +2737,11 @@
       <c r="X22" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:32">
+      <c r="Y22" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33">
       <c r="A23" s="2" t="s">
         <v>37</v>
       </c>
@@ -2732,7 +2782,7 @@
         <v>24</v>
       </c>
       <c r="N23" s="2">
-        <f>(I23*0.001)</f>
+        <f t="shared" si="12"/>
         <v>0.05</v>
       </c>
       <c r="O23">
@@ -2741,21 +2791,20 @@
       <c r="P23">
         <v>0.13700000000000001</v>
       </c>
-      <c r="R23">
-        <f t="shared" si="6"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+      <c r="S23">
+        <f t="shared" si="7"/>
         <v>2.8700000000000002E-3</v>
       </c>
-      <c r="S23">
-        <f t="shared" si="2"/>
+      <c r="T23">
+        <f t="shared" si="3"/>
         <v>6.8500000000000011E-3</v>
       </c>
-      <c r="T23" s="5">
-        <f t="shared" si="7"/>
+      <c r="U23" s="5">
+        <f t="shared" si="8"/>
         <v>9.7200000000000012E-3</v>
       </c>
-      <c r="U23" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="V23" s="4" t="s">
         <v>24</v>
       </c>
@@ -2765,8 +2814,11 @@
       <c r="X23" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:32">
+      <c r="Y23" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33">
       <c r="A24" s="2" t="s">
         <v>37</v>
       </c>
@@ -2807,7 +2859,7 @@
         <v>24</v>
       </c>
       <c r="N24" s="2">
-        <f>(I24*0.001)</f>
+        <f t="shared" si="12"/>
         <v>0.05</v>
       </c>
       <c r="O24">
@@ -2816,21 +2868,20 @@
       <c r="P24">
         <v>0.19</v>
       </c>
-      <c r="R24">
-        <f t="shared" si="6"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="S24">
+        <f t="shared" si="7"/>
         <v>3.2975000000000001E-3</v>
       </c>
-      <c r="S24">
-        <f t="shared" si="2"/>
+      <c r="T24">
+        <f t="shared" si="3"/>
         <v>9.5000000000000015E-3</v>
       </c>
-      <c r="T24" s="5">
-        <f t="shared" si="7"/>
+      <c r="U24" s="5">
+        <f t="shared" si="8"/>
         <v>1.2797500000000002E-2</v>
       </c>
-      <c r="U24" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="V24" s="4" t="s">
         <v>24</v>
       </c>
@@ -2840,8 +2891,11 @@
       <c r="X24" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:32">
+      <c r="Y24" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33">
       <c r="A25" s="2" t="s">
         <v>38</v>
       </c>
@@ -2882,7 +2936,7 @@
         <v>24</v>
       </c>
       <c r="N25" s="2">
-        <f>(I25*0.001)</f>
+        <f t="shared" si="12"/>
         <v>0.05</v>
       </c>
       <c r="O25" s="3" t="s">
@@ -2891,18 +2945,19 @@
       <c r="P25" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
       <c r="S25" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="U25" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:32">
+      <c r="T25" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="V25" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33">
       <c r="A26" s="2" t="s">
         <v>38</v>
       </c>
@@ -2943,7 +2998,7 @@
         <v>24</v>
       </c>
       <c r="N26" s="2">
-        <f>(I26*0.001)</f>
+        <f t="shared" si="12"/>
         <v>0.05</v>
       </c>
       <c r="O26" s="3" t="s">
@@ -2952,21 +3007,22 @@
       <c r="P26" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
       <c r="S26" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="U26" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB26" t="s">
+      <c r="T26" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="V26" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC26" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:32">
+    <row r="27" spans="1:33">
       <c r="A27" s="2" t="s">
         <v>38</v>
       </c>
@@ -3007,7 +3063,7 @@
         <v>24</v>
       </c>
       <c r="N27" s="2">
-        <f>(I27*0.001)</f>
+        <f t="shared" si="12"/>
         <v>0.05</v>
       </c>
       <c r="O27" s="3" t="s">
@@ -3016,525 +3072,528 @@
       <c r="P27" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Q27" s="3"/>
-      <c r="R27" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
       <c r="S27" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="U27" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:32">
-      <c r="AA28" t="s">
+      <c r="T27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="V27" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33">
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="AB28" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:32">
-      <c r="X30" t="s">
+    <row r="30" spans="1:33">
+      <c r="Y30" t="s">
         <v>54</v>
       </c>
-      <c r="Y30" t="s">
+      <c r="Z30" t="s">
         <v>56</v>
       </c>
-      <c r="AA30" t="s">
+      <c r="AB30" t="s">
         <v>52</v>
       </c>
-      <c r="AD30" t="s">
+      <c r="AE30" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:32">
-      <c r="U31" t="s">
+    <row r="31" spans="1:33">
+      <c r="V31" t="s">
         <v>48</v>
       </c>
-      <c r="AA31" t="s">
+      <c r="AB31" t="s">
         <v>49</v>
       </c>
-      <c r="AB31" t="s">
+      <c r="AC31" t="s">
         <v>50</v>
       </c>
-      <c r="AC31" t="s">
+      <c r="AD31" t="s">
         <v>51</v>
       </c>
-      <c r="AD31" t="s">
+      <c r="AE31" t="s">
         <v>57</v>
       </c>
-      <c r="AE31" t="s">
+      <c r="AF31" t="s">
         <v>58</v>
       </c>
-      <c r="AF31" t="s">
+      <c r="AG31" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:32">
-      <c r="X32" t="s">
+    <row r="32" spans="1:33">
+      <c r="Y32" t="s">
         <v>53</v>
       </c>
-      <c r="Y32" t="s">
+      <c r="Z32" t="s">
         <v>55</v>
       </c>
-      <c r="Z32" t="s">
+      <c r="AA32" t="s">
         <v>47</v>
       </c>
-      <c r="AA32" s="1" t="s">
+      <c r="AB32" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AB32" s="1" t="s">
+      <c r="AC32" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AC32" s="1" t="s">
+      <c r="AD32" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AD32" s="1" t="s">
+      <c r="AE32" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AE32" s="1" t="s">
+      <c r="AF32" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AF32" s="1" t="s">
+      <c r="AG32" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="21:32">
-      <c r="U33" s="2" t="s">
+    <row r="33" spans="22:33">
+      <c r="V33" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="V33" s="2" t="s">
+      <c r="W33" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="W33" s="3">
-        <v>41823</v>
-      </c>
-      <c r="X33" s="6">
+      <c r="X33" s="3">
+        <v>41823</v>
+      </c>
+      <c r="Y33" s="6">
         <v>1.47</v>
       </c>
-      <c r="Y33">
+      <c r="Z33">
         <v>10</v>
       </c>
-      <c r="Z33">
+      <c r="AA33">
         <v>7</v>
       </c>
-      <c r="AA33">
-        <f>(V12-V2)/$Z33</f>
+      <c r="AB33">
+        <f>(W12-W2)/$AA33</f>
         <v>2.481978476535137E-3</v>
       </c>
-      <c r="AB33">
-        <f>(W12-W2)/$Z33</f>
+      <c r="AC33">
+        <f>(X12-X2)/$AA33</f>
         <v>-2.0924496855919991E-3</v>
       </c>
-      <c r="AC33">
-        <f>(X12-X2)/$Z33</f>
+      <c r="AD33">
+        <f>(Y12-Y2)/$AA33</f>
         <v>3.8952879094313845E-4</v>
       </c>
-      <c r="AD33">
-        <f>AA33*$X33*$Y33*10000</f>
+      <c r="AE33">
+        <f t="shared" ref="AE33:AE42" si="13">AB33*$Y33*$Z33*10000</f>
         <v>364.85083605066512</v>
       </c>
-      <c r="AE33">
-        <f>AB33*$X33*$Y33*10000</f>
+      <c r="AF33">
+        <f t="shared" ref="AF33:AF42" si="14">AC33*$Y33*$Z33*10000</f>
         <v>-307.59010378202385</v>
       </c>
-      <c r="AF33">
-        <f>AC33*$X33*$Y33*10000</f>
+      <c r="AG33">
+        <f t="shared" ref="AG33:AG42" si="15">AD33*$Y33*$Z33*10000</f>
         <v>57.260732268641348</v>
       </c>
     </row>
-    <row r="34" spans="21:32">
-      <c r="U34" s="2" t="s">
+    <row r="34" spans="22:33">
+      <c r="V34" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="V34" s="2" t="s">
+      <c r="W34" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="W34" s="3">
-        <v>41823</v>
-      </c>
-      <c r="X34" s="6">
+      <c r="X34" s="3">
+        <v>41823</v>
+      </c>
+      <c r="Y34" s="6">
         <v>1.47</v>
       </c>
-      <c r="Y34">
+      <c r="Z34">
         <v>10</v>
       </c>
-      <c r="Z34">
+      <c r="AA34">
         <v>7</v>
       </c>
-      <c r="AA34">
-        <f>(V13-V3)/$Z34</f>
+      <c r="AB34">
+        <f>(W13-W3)/$AA34</f>
         <v>1.6403934193131211E-3</v>
       </c>
-      <c r="AB34">
-        <f t="shared" ref="AB33:AC42" si="11">(W13-W3)/$Z34</f>
+      <c r="AC34">
+        <f t="shared" ref="AC34:AD42" si="16">(X13-X3)/$AA34</f>
         <v>-1.7693666592214679E-4</v>
       </c>
-      <c r="AC34">
-        <f t="shared" si="11"/>
+      <c r="AD34">
+        <f t="shared" si="16"/>
         <v>1.4634567533909747E-3</v>
       </c>
-      <c r="AD34">
-        <f>AA34*$X34*$Y34*10000</f>
+      <c r="AE34">
+        <f t="shared" si="13"/>
         <v>241.13783263902883</v>
       </c>
-      <c r="AE34">
-        <f>AB34*$X34*$Y34*10000</f>
+      <c r="AF34">
+        <f t="shared" si="14"/>
         <v>-26.009689890555574</v>
       </c>
-      <c r="AF34">
-        <f>AC34*$X34*$Y34*10000</f>
+      <c r="AG34">
+        <f t="shared" si="15"/>
         <v>215.12814274847327</v>
       </c>
     </row>
-    <row r="35" spans="21:32">
-      <c r="U35" s="2" t="s">
+    <row r="35" spans="22:33">
+      <c r="V35" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="V35" s="2" t="s">
+      <c r="W35" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="W35" s="3">
-        <v>41823</v>
-      </c>
-      <c r="X35" s="6">
+      <c r="X35" s="3">
+        <v>41823</v>
+      </c>
+      <c r="Y35" s="6">
         <v>1.47</v>
       </c>
-      <c r="Y35">
+      <c r="Z35">
         <v>10</v>
       </c>
-      <c r="Z35">
+      <c r="AA35">
         <v>7</v>
       </c>
-      <c r="AA35">
-        <f>(V14-V4)/$Z35</f>
+      <c r="AB35">
+        <f>(W14-W4)/$AA35</f>
         <v>3.3884079603662865E-3</v>
       </c>
-      <c r="AB35">
-        <f t="shared" si="11"/>
+      <c r="AC35">
+        <f t="shared" si="16"/>
         <v>-1.9222345205026443E-3</v>
       </c>
-      <c r="AC35">
-        <f t="shared" si="11"/>
+      <c r="AD35">
+        <f t="shared" si="16"/>
         <v>1.4661734398636432E-3</v>
       </c>
-      <c r="AD35">
-        <f>AA35*$X35*$Y35*10000</f>
+      <c r="AE35">
+        <f t="shared" si="13"/>
         <v>498.09597017384408</v>
       </c>
-      <c r="AE35">
-        <f>AB35*$X35*$Y35*10000</f>
+      <c r="AF35">
+        <f t="shared" si="14"/>
         <v>-282.5684745138887</v>
       </c>
-      <c r="AF35">
-        <f>AC35*$X35*$Y35*10000</f>
+      <c r="AG35">
+        <f t="shared" si="15"/>
         <v>215.52749565995555</v>
       </c>
     </row>
-    <row r="36" spans="21:32">
-      <c r="U36" s="2" t="s">
+    <row r="36" spans="22:33">
+      <c r="V36" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="V36" s="2" t="s">
+      <c r="W36" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W36" s="3">
-        <v>41823</v>
-      </c>
-      <c r="X36" s="6">
+      <c r="X36" s="3">
+        <v>41823</v>
+      </c>
+      <c r="Y36" s="6">
         <v>1.47</v>
       </c>
-      <c r="Y36">
+      <c r="Z36">
         <v>10</v>
       </c>
-      <c r="Z36">
+      <c r="AA36">
         <v>7</v>
       </c>
-      <c r="AA36">
-        <f t="shared" ref="AA36:AA42" si="12">(V15-V5)/$Z36</f>
+      <c r="AB36">
+        <f t="shared" ref="AB36:AB42" si="17">(W15-W5)/$AA36</f>
         <v>3.2599526540879088E-3</v>
       </c>
-      <c r="AB36">
-        <f t="shared" si="11"/>
+      <c r="AC36">
+        <f t="shared" si="16"/>
         <v>-3.4992880635282783E-3</v>
       </c>
-      <c r="AC36">
-        <f t="shared" si="11"/>
+      <c r="AD36">
+        <f t="shared" si="16"/>
         <v>-2.3933540944036974E-4</v>
       </c>
-      <c r="AD36">
-        <f>AA36*$X36*$Y36*10000</f>
+      <c r="AE36">
+        <f t="shared" si="13"/>
         <v>479.21304015092261</v>
       </c>
-      <c r="AE36">
-        <f>AB36*$X36*$Y36*10000</f>
+      <c r="AF36">
+        <f t="shared" si="14"/>
         <v>-514.39534533865697</v>
       </c>
-      <c r="AF36">
-        <f>AC36*$X36*$Y36*10000</f>
+      <c r="AG36">
+        <f t="shared" si="15"/>
         <v>-35.182305187734343</v>
       </c>
     </row>
-    <row r="37" spans="21:32">
-      <c r="U37" s="2" t="s">
+    <row r="37" spans="22:33">
+      <c r="V37" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="V37" s="2" t="s">
+      <c r="W37" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W37" s="3">
-        <v>41823</v>
-      </c>
-      <c r="X37" s="6">
+      <c r="X37" s="3">
+        <v>41823</v>
+      </c>
+      <c r="Y37" s="6">
         <v>1.47</v>
       </c>
-      <c r="Y37">
+      <c r="Z37">
         <v>10</v>
       </c>
-      <c r="Z37">
+      <c r="AA37">
         <v>7</v>
       </c>
-      <c r="AA37">
-        <f>(V16-V6)/$Z37</f>
+      <c r="AB37">
+        <f>(W16-W6)/$AA37</f>
         <v>2.0646205023859615E-3</v>
       </c>
-      <c r="AB37">
-        <f t="shared" si="11"/>
+      <c r="AC37">
+        <f t="shared" si="16"/>
         <v>-5.6453553595415466E-4</v>
       </c>
-      <c r="AC37">
-        <f>(X16-X6)/$Z37</f>
+      <c r="AD37">
+        <f>(Y16-Y6)/$AA37</f>
         <v>1.5000849664318072E-3</v>
       </c>
-      <c r="AD37">
-        <f>AA37*$X37*$Y37*10000</f>
+      <c r="AE37">
+        <f t="shared" si="13"/>
         <v>303.49921385073634</v>
       </c>
-      <c r="AE37">
-        <f>AB37*$X37*$Y37*10000</f>
+      <c r="AF37">
+        <f t="shared" si="14"/>
         <v>-82.986723785260736</v>
       </c>
-      <c r="AF37">
-        <f>AC37*$X37*$Y37*10000</f>
+      <c r="AG37">
+        <f t="shared" si="15"/>
         <v>220.51249006547567</v>
       </c>
     </row>
-    <row r="38" spans="21:32">
-      <c r="U38" s="2" t="s">
+    <row r="38" spans="22:33">
+      <c r="V38" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="V38" s="2" t="s">
+      <c r="W38" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="W38" s="3">
-        <v>41823</v>
-      </c>
-      <c r="X38" s="6">
+      <c r="X38" s="3">
+        <v>41823</v>
+      </c>
+      <c r="Y38" s="6">
         <v>1.36</v>
       </c>
-      <c r="Y38">
+      <c r="Z38">
         <v>10</v>
       </c>
-      <c r="Z38">
+      <c r="AA38">
         <v>7</v>
       </c>
-      <c r="AA38">
-        <f t="shared" si="12"/>
+      <c r="AB38">
+        <f t="shared" si="17"/>
         <v>9.4515495139359999E-4</v>
       </c>
-      <c r="AB38">
-        <f t="shared" si="11"/>
+      <c r="AC38">
+        <f t="shared" si="16"/>
         <v>-3.9204037787169809E-5</v>
       </c>
-      <c r="AC38">
-        <f t="shared" si="11"/>
+      <c r="AD38">
+        <f t="shared" si="16"/>
         <v>9.059509136064304E-4</v>
       </c>
-      <c r="AD38">
-        <f>AA38*$X38*$Y38*10000</f>
+      <c r="AE38">
+        <f t="shared" si="13"/>
         <v>128.5410733895296</v>
       </c>
-      <c r="AE38">
-        <f>AB38*$X38*$Y38*10000</f>
+      <c r="AF38">
+        <f t="shared" si="14"/>
         <v>-5.331749139055094</v>
       </c>
-      <c r="AF38">
-        <f>AC38*$X38*$Y38*10000</f>
+      <c r="AG38">
+        <f t="shared" si="15"/>
         <v>123.20932425047455</v>
       </c>
     </row>
-    <row r="39" spans="21:32">
-      <c r="U39" s="2" t="s">
+    <row r="39" spans="22:33">
+      <c r="V39" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="V39" s="2" t="s">
+      <c r="W39" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="W39" s="3">
-        <v>41823</v>
-      </c>
-      <c r="X39" s="6">
+      <c r="X39" s="3">
+        <v>41823</v>
+      </c>
+      <c r="Y39" s="6">
         <v>1.36</v>
       </c>
-      <c r="Y39">
+      <c r="Z39">
         <v>10</v>
       </c>
-      <c r="Z39">
+      <c r="AA39">
         <v>7</v>
       </c>
-      <c r="AA39">
-        <f>(V18-V8)/$Z39</f>
+      <c r="AB39">
+        <f>(W18-W8)/$AA39</f>
         <v>4.9504449824594086E-4</v>
       </c>
-      <c r="AB39">
-        <f t="shared" si="11"/>
+      <c r="AC39">
+        <f t="shared" si="16"/>
         <v>1.0454408777710422E-5</v>
       </c>
-      <c r="AC39">
-        <f t="shared" si="11"/>
+      <c r="AD39">
+        <f t="shared" si="16"/>
         <v>5.0549890702365123E-4</v>
       </c>
-      <c r="AD39">
-        <f>AA39*$X39*$Y39*10000</f>
+      <c r="AE39">
+        <f t="shared" si="13"/>
         <v>67.326051761447957</v>
       </c>
-      <c r="AE39">
-        <f>AB39*$X39*$Y39*10000</f>
+      <c r="AF39">
+        <f t="shared" si="14"/>
         <v>1.4217995937686176</v>
       </c>
-      <c r="AF39">
-        <f>AC39*$X39*$Y39*10000</f>
+      <c r="AG39">
+        <f t="shared" si="15"/>
         <v>68.747851355216568</v>
       </c>
     </row>
-    <row r="40" spans="21:32">
-      <c r="U40" s="2" t="s">
+    <row r="40" spans="22:33">
+      <c r="V40" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="V40" s="2" t="s">
+      <c r="W40" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="W40" s="3">
-        <v>41823</v>
-      </c>
-      <c r="X40" s="6">
+      <c r="X40" s="3">
+        <v>41823</v>
+      </c>
+      <c r="Y40" s="6">
         <v>1.36</v>
       </c>
-      <c r="Y40">
+      <c r="Z40">
         <v>10</v>
       </c>
-      <c r="Z40">
+      <c r="AA40">
         <v>7</v>
       </c>
-      <c r="AA40">
-        <f t="shared" si="12"/>
+      <c r="AB40">
+        <f t="shared" si="17"/>
         <v>8.0267373638902696E-4</v>
       </c>
-      <c r="AB40">
-        <f>(W19-W9)/$Z40</f>
+      <c r="AC40">
+        <f>(X19-X9)/$AA40</f>
         <v>-6.6147232495212077E-5</v>
       </c>
-      <c r="AC40">
-        <f>(X19-X9)/$Z40</f>
+      <c r="AD40">
+        <f>(Y19-Y9)/$AA40</f>
         <v>7.3652650389381528E-4</v>
       </c>
-      <c r="AD40">
-        <f>AA40*$X40*$Y40*10000</f>
+      <c r="AE40">
+        <f t="shared" si="13"/>
         <v>109.16362814890768</v>
       </c>
-      <c r="AE40">
-        <f>AB40*$X40*$Y40*10000</f>
+      <c r="AF40">
+        <f t="shared" si="14"/>
         <v>-8.9960236193488434</v>
       </c>
-      <c r="AF40">
-        <f>AC40*$X40*$Y40*10000</f>
+      <c r="AG40">
+        <f t="shared" si="15"/>
         <v>100.16760452955887</v>
       </c>
     </row>
-    <row r="41" spans="21:32">
-      <c r="U41" s="2" t="s">
+    <row r="41" spans="22:33">
+      <c r="V41" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="V41" s="2" t="s">
+      <c r="W41" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W41" s="3">
-        <v>41823</v>
-      </c>
-      <c r="X41" s="6">
+      <c r="X41" s="3">
+        <v>41823</v>
+      </c>
+      <c r="Y41" s="6">
         <v>1.36</v>
       </c>
-      <c r="Y41">
+      <c r="Z41">
         <v>10</v>
       </c>
-      <c r="Z41">
+      <c r="AA41">
         <v>7</v>
       </c>
-      <c r="AA41">
-        <f t="shared" si="12"/>
+      <c r="AB41">
+        <f t="shared" si="17"/>
         <v>1.7677544317272213E-3</v>
       </c>
-      <c r="AB41">
-        <f t="shared" si="11"/>
+      <c r="AC41">
+        <f t="shared" si="16"/>
         <v>3.9271049425395706E-5</v>
       </c>
-      <c r="AC41">
-        <f t="shared" si="11"/>
+      <c r="AD41">
+        <f t="shared" si="16"/>
         <v>1.8070254811526167E-3</v>
       </c>
-      <c r="AD41">
-        <f>AA41*$X41*$Y41*10000</f>
+      <c r="AE41">
+        <f t="shared" si="13"/>
         <v>240.41460271490212</v>
       </c>
-      <c r="AE41">
-        <f>AB41*$X41*$Y41*10000</f>
+      <c r="AF41">
+        <f t="shared" si="14"/>
         <v>5.3408627218538172</v>
       </c>
-      <c r="AF41">
-        <f>AC41*$X41*$Y41*10000</f>
+      <c r="AG41">
+        <f t="shared" si="15"/>
         <v>245.75546543675591</v>
       </c>
     </row>
-    <row r="42" spans="21:32">
-      <c r="U42" s="2" t="s">
+    <row r="42" spans="22:33">
+      <c r="V42" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="V42" s="2" t="s">
+      <c r="W42" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W42" s="3">
-        <v>41823</v>
-      </c>
-      <c r="X42" s="6">
+      <c r="X42" s="3">
+        <v>41823</v>
+      </c>
+      <c r="Y42" s="6">
         <v>1.36</v>
       </c>
-      <c r="Y42">
+      <c r="Z42">
         <v>10</v>
       </c>
-      <c r="Z42">
+      <c r="AA42">
         <v>7</v>
       </c>
-      <c r="AA42">
-        <f t="shared" si="12"/>
+      <c r="AB42">
+        <f t="shared" si="17"/>
         <v>1.4668708670194375E-4</v>
       </c>
-      <c r="AB42">
-        <f t="shared" si="11"/>
+      <c r="AC42">
+        <f t="shared" si="16"/>
         <v>2.1819664181582771E-5</v>
       </c>
-      <c r="AC42">
-        <f t="shared" si="11"/>
+      <c r="AD42">
+        <f t="shared" si="16"/>
         <v>1.6850675088352679E-4</v>
       </c>
-      <c r="AD42">
-        <f>AA42*$X42*$Y42*10000</f>
+      <c r="AE42">
+        <f t="shared" si="13"/>
         <v>19.949443791464354</v>
       </c>
-      <c r="AE42">
-        <f>AB42*$X42*$Y42*10000</f>
+      <c r="AF42">
+        <f t="shared" si="14"/>
         <v>2.967474328695257</v>
       </c>
-      <c r="AF42">
-        <f>AC42*$X42*$Y42*10000</f>
+      <c r="AG42">
+        <f t="shared" si="15"/>
         <v>22.916918120159643</v>
       </c>
     </row>

</xml_diff>